<commit_message>
Modificato sistema di creazione reazioni
</commit_message>
<xml_diff>
--- a/GillesPy2/ProvaEvento/output.xlsx
+++ b/GillesPy2/ProvaEvento/output.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,20 +446,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>AB</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>AC</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>BC</t>
         </is>
@@ -467,266 +462,233 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="n">
         <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>61.95</v>
+        <v>60.95</v>
       </c>
       <c r="D2" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" t="n">
         <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>62.9</v>
+        <v>61.9</v>
       </c>
       <c r="D3" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>63.85</v>
+        <v>62.85</v>
       </c>
       <c r="D4" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
-      </c>
-      <c r="G4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C5" t="n">
-        <v>64.8</v>
+        <v>63.8</v>
       </c>
       <c r="D5" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
-      </c>
-      <c r="G5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C6" t="n">
-        <v>65.75</v>
+        <v>64.75</v>
       </c>
       <c r="D6" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B7" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>67.7</v>
+        <v>65.7</v>
       </c>
       <c r="D7" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B8" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="n">
-        <v>68.65000000000001</v>
+        <v>66.65000000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
-      </c>
-      <c r="G8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B9" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="n">
-        <v>71.59999999999999</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B10" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" t="n">
-        <v>74.55</v>
+        <v>68.55</v>
       </c>
       <c r="D10" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>35</v>
+        <v>42.95</v>
       </c>
       <c r="B11" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>75.5</v>
+        <v>69.5</v>
       </c>
       <c r="D11" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
-      </c>
-      <c r="G11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>32</v>
+        <v>43.9</v>
       </c>
       <c r="B12" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C12" t="n">
-        <v>80.45</v>
+        <v>70.45</v>
       </c>
       <c r="D12" t="n">
-        <v>53.1583</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
-      </c>
-      <c r="G12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>44.85</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -735,2034 +697,1767 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>44.8</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>71.34999999999999</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>45.75</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>72.3</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>45.7</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>72.25</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>46.65</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>73.2</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>74.15000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>47.55</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>48.5</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>76.05</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>48.45</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>49.4</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>76.95</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>50.35</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>78.84999999999999</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>51.25</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>77.8</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0</v>
+        <v>52.2</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>78.75</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0</v>
+        <v>53.15</v>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>79.7</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0</v>
+        <v>54.1</v>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>80.65000000000001</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0</v>
+        <v>53.05</v>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>79.59999999999999</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>80.55</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0</v>
+        <v>54.95</v>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>81.5</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0</v>
+        <v>55.9</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>81.45</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0</v>
+        <v>56.85</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>82.40000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0</v>
+        <v>57.8</v>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>83.34999999999999</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0</v>
+        <v>58.75</v>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>84.3</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0</v>
+        <v>59.7</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>85.25</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0</v>
+        <v>60.65</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>45.95</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>86.2</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0</v>
+        <v>61.6</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>46.9</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>87.15000000000001</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0</v>
+        <v>62.55</v>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>47.85</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>88.09999999999999</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0</v>
+        <v>63.5</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>48.8</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>89.05</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0</v>
+        <v>64.45</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>49.75</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0</v>
+        <v>63.4</v>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>49.7</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>89.95</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0</v>
+        <v>64.34999999999999</v>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
+        <v>50.65</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0</v>
+        <v>65.3</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>51.6</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>91.84999999999999</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0</v>
+        <v>66.25</v>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>52.55</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>92.8</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0</v>
+        <v>66.2</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>53.5</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>92.75</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0</v>
+        <v>65.15000000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>53.45</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>92.7</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>53.4</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>93.65000000000001</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0</v>
+        <v>66.05</v>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>53.35</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>54.3</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>94.55</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0</v>
+        <v>67.95</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>55.25</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>95.5</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>56.2</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>95.45</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0</v>
+        <v>67.84999999999999</v>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>57.15</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0</v>
+        <v>68.8</v>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>58.1</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>96.34999999999999</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0</v>
+        <v>69.75</v>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>59.05</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>97.3</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0</v>
+        <v>70.7</v>
       </c>
       <c r="B56" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>97.25</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0</v>
+        <v>71.65000000000001</v>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>59.95</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>98.2</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>60.9</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>99.15000000000001</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0</v>
+        <v>73.55</v>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>61.85</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>100.1</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0</v>
+        <v>74.5</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>62.8</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>101.05</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0</v>
+        <v>75.45</v>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>63.75</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>0</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>64.7</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>102.95</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0</v>
+        <v>77.34999999999999</v>
       </c>
       <c r="B63" t="n">
-        <v>0</v>
+        <v>65.65000000000001</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>103.9</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0</v>
+        <v>77.3</v>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>103.85</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0</v>
+        <v>78.25</v>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>67.55</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>104.8</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0</v>
+        <v>79.2</v>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>68.5</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>105.75</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0</v>
+        <v>80.15000000000001</v>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>69.45</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>106.7</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0</v>
+        <v>79.09999999999999</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>106.65</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F68" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0</v>
+        <v>78.05</v>
       </c>
       <c r="B69" t="n">
-        <v>0</v>
+        <v>68.34999999999999</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>107.6</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>69.3</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>108.55</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0</v>
+        <v>78.95</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>70.25</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>108.5</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
-      </c>
-      <c r="G71" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>70.2</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>108.45</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>0</v>
+        <v>80.84999999999999</v>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>71.15000000000001</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>109.4</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
-      </c>
-      <c r="G73" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0</v>
+        <v>81.7</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>72.09999999999999</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>110.25</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0</v>
+        <v>82.55</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>73.05</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>111.1</v>
       </c>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="F75" t="n">
-        <v>0</v>
-      </c>
-      <c r="G75" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0</v>
+        <v>82.40000000000001</v>
       </c>
       <c r="B76" t="n">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>111.95</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
-      </c>
-      <c r="G76" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0</v>
+        <v>83.25</v>
       </c>
       <c r="B77" t="n">
-        <v>0</v>
+        <v>73.95</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>112.8</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>12.4</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
-      </c>
-      <c r="G77" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0</v>
+        <v>84.09999999999999</v>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>113.65</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G78" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0</v>
+        <v>83.95</v>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>74.84999999999999</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>114.5</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>12.6</v>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
-      </c>
-      <c r="G79" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0</v>
+        <v>84.8</v>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>75.8</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>115.35</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>12.7</v>
       </c>
       <c r="F80" t="n">
-        <v>0</v>
-      </c>
-      <c r="G80" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0</v>
+        <v>85.65000000000001</v>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>76.75</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>116.2</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>12.8</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
-      </c>
-      <c r="G81" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0</v>
+        <v>86.5</v>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>77.7</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>117.05</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
-      </c>
-      <c r="G82" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0</v>
+        <v>87.34999999999999</v>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>78.65000000000001</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>117.9</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
-      </c>
-      <c r="G83" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0</v>
+        <v>88.2</v>
       </c>
       <c r="B84" t="n">
-        <v>0</v>
+        <v>79.59999999999999</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>118.75</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="F84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G84" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0</v>
+        <v>88.05</v>
       </c>
       <c r="B85" t="n">
-        <v>0</v>
+        <v>79.55</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>119.6</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
-      </c>
-      <c r="G85" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0</v>
+        <v>88.90000000000001</v>
       </c>
       <c r="B86" t="n">
-        <v>0</v>
+        <v>80.5</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>120.45</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="F86" t="n">
-        <v>0</v>
-      </c>
-      <c r="G86" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0</v>
+        <v>89.65000000000001</v>
       </c>
       <c r="B87" t="n">
-        <v>0</v>
+        <v>81.34999999999999</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>121.3</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>13.4</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
-      </c>
-      <c r="G87" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>82.2</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>122.15</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="F88" t="n">
-        <v>0</v>
-      </c>
-      <c r="G88" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0</v>
+        <v>91.15000000000001</v>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>83.05</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>13.6</v>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
-      </c>
-      <c r="G89" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0</v>
+        <v>91.90000000000001</v>
       </c>
       <c r="B90" t="n">
-        <v>0</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>123.85</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>12.4</v>
       </c>
       <c r="E90" t="n">
-        <v>0</v>
+        <v>13.7</v>
       </c>
       <c r="F90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G90" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0</v>
+        <v>92.65000000000001</v>
       </c>
       <c r="B91" t="n">
-        <v>0</v>
+        <v>84.75</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>124.7</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>13.8</v>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
-      </c>
-      <c r="G91" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0</v>
+        <v>93.40000000000001</v>
       </c>
       <c r="B92" t="n">
-        <v>0</v>
+        <v>85.59999999999999</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>125.55</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>12.6</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>13.9</v>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G92" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0</v>
+        <v>94.15000000000001</v>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>86.45</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>126.4</v>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>12.7</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F93" t="n">
-        <v>0</v>
-      </c>
-      <c r="G93" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0</v>
+        <v>94.90000000000001</v>
       </c>
       <c r="B94" t="n">
-        <v>0</v>
+        <v>87.3</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>127.25</v>
       </c>
       <c r="D94" t="n">
-        <v>0</v>
+        <v>12.8</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>14.1</v>
       </c>
       <c r="F94" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0</v>
+        <v>95.65000000000001</v>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>88.15000000000001</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>128.1</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>14.2</v>
       </c>
       <c r="F95" t="n">
-        <v>0</v>
-      </c>
-      <c r="G95" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0</v>
+        <v>96.40000000000001</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>128.95</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>14.3</v>
       </c>
       <c r="F96" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0</v>
+        <v>97.15000000000001</v>
       </c>
       <c r="B97" t="n">
-        <v>0</v>
+        <v>89.84999999999999</v>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>129.8</v>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="E97" t="n">
-        <v>0</v>
+        <v>14.4</v>
       </c>
       <c r="F97" t="n">
-        <v>0</v>
-      </c>
-      <c r="G97" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0</v>
+        <v>97.90000000000001</v>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>90.7</v>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>130.65</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="E98" t="n">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="F98" t="n">
-        <v>0</v>
-      </c>
-      <c r="G98" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0</v>
+        <v>98.65000000000001</v>
       </c>
       <c r="B99" t="n">
-        <v>0</v>
+        <v>91.55</v>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>131.5</v>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="F99" t="n">
-        <v>0</v>
-      </c>
-      <c r="G99" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="B100" t="n">
-        <v>0</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>132.35</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>13.4</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>14.7</v>
       </c>
       <c r="F100" t="n">
-        <v>0</v>
-      </c>
-      <c r="G100" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0</v>
+        <v>50.15</v>
       </c>
       <c r="B101" t="n">
-        <v>0</v>
+        <v>93.25</v>
       </c>
       <c r="C101" t="n">
-        <v>0</v>
+        <v>133.2</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>14.8</v>
       </c>
       <c r="F101" t="n">
-        <v>0</v>
-      </c>
-      <c r="G101" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>